<commit_message>
create app of analysis
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icbfsfood-my.sharepoint.com/personal/scatalanv_icbfs_cl/Documents/posicionamiento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4341" documentId="11_AD4D2F04E46CFB4ACB3E200E4DD7FD88683EDF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86C8A5A3-4C96-48F6-B97B-B08D472681F6}"/>
+  <xr:revisionPtr revIDLastSave="4350" documentId="11_AD4D2F04E46CFB4ACB3E200E4DD7FD88683EDF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A0B1BA0-2D43-4923-85DD-61E9011C5DF4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22759,8 +22759,8 @@
   <dimension ref="A1:L939"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A479" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L820" sqref="L820"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51789,6 +51789,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L939" xr:uid="{D507D2F6-219C-44EE-8F13-68F6A84834B5}"/>
   <hyperlinks>
     <hyperlink ref="F482" r:id="rId1" xr:uid="{B8A99D23-CCD3-4507-B1C1-F297A3CD9A42}"/>
     <hyperlink ref="F484" r:id="rId2" xr:uid="{BEBB2D9E-08F4-40D9-8C60-12C2F1BA1BE7}"/>

</xml_diff>

<commit_message>
updated base with bidfood info
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icbfsfood-my.sharepoint.com/personal/scatalanv_icbfs_cl/Documents/posicionamiento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4352" documentId="11_AD4D2F04E46CFB4ACB3E200E4DD7FD88683EDF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87F611AC-D297-4397-84C1-AB91217DA974}"/>
+  <xr:revisionPtr revIDLastSave="4630" documentId="11_AD4D2F04E46CFB4ACB3E200E4DD7FD88683EDF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD80AE7A-A813-4683-9EAC-C9CC482171B8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">base!$A$1:$L$939</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">base!$A$1:$L$993</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4084" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4300" uniqueCount="1112">
   <si>
     <t>CÓDIGO</t>
   </si>
@@ -3250,6 +3250,135 @@
   </si>
   <si>
     <t>otros</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/304460002</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/300404007</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/300406003</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/304420001</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/204180025</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/200250039</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/202730011</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/200201032</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/202730014</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/202730039</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/202720006</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/204310013</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/202730017</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/202720033</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/204310008</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/100753002</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/304430000</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/100004001</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/202910013</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/202910014</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/304760227</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/304760001</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/304760108</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/200455004</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/200455003</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/101353011</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/101353038</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/103880017</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/300353024</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/202730070</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/200200010</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/101403002</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/101400001</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/103070006</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/101403004</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/200460023</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/200460018</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/203210096</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/300407004</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/300407001</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/100050007</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/202910045</t>
+  </si>
+  <si>
+    <t>https://www.mybidfood.cl/#/products/detail/200300002</t>
   </si>
 </sst>
 </file>
@@ -3316,7 +3445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3330,6 +3459,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -22752,11 +22884,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D507D2F6-219C-44EE-8F13-68F6A84834B5}">
-  <dimension ref="A1:L939"/>
+  <dimension ref="A1:L993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I259" sqref="I259"/>
+      <pane ySplit="1" topLeftCell="A950" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E952" sqref="E952"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51782,6 +51914,1684 @@
       </c>
       <c r="L939" t="s">
         <v>1065</v>
+      </c>
+    </row>
+    <row r="940" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A940">
+        <v>104500500</v>
+      </c>
+      <c r="B940" t="s">
+        <v>73</v>
+      </c>
+      <c r="C940" s="1"/>
+      <c r="E940" t="s">
+        <v>584</v>
+      </c>
+      <c r="F940" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="G940">
+        <v>6153</v>
+      </c>
+      <c r="H940">
+        <v>1</v>
+      </c>
+      <c r="I940" s="5">
+        <f>G940/H940</f>
+        <v>6153</v>
+      </c>
+      <c r="J940" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L940" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="941" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A941">
+        <v>104519930</v>
+      </c>
+      <c r="B941" t="s">
+        <v>74</v>
+      </c>
+      <c r="C941" s="1"/>
+      <c r="E941" t="s">
+        <v>584</v>
+      </c>
+      <c r="F941" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G941">
+        <v>7431</v>
+      </c>
+      <c r="H941">
+        <f>_xlfn.XLOOKUP(A941,'[1]BD LP'!$B:$B,'[1]BD LP'!$AC:$AC)</f>
+        <v>1</v>
+      </c>
+      <c r="I941" s="5">
+        <f t="shared" ref="I941:I950" si="35">G941/H941</f>
+        <v>7431</v>
+      </c>
+      <c r="J941" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L941" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="942" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A942">
+        <v>104520790</v>
+      </c>
+      <c r="B942" t="s">
+        <v>75</v>
+      </c>
+      <c r="C942" s="1"/>
+      <c r="E942" t="s">
+        <v>584</v>
+      </c>
+      <c r="F942" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G942">
+        <v>7932</v>
+      </c>
+      <c r="H942">
+        <v>1</v>
+      </c>
+      <c r="I942" s="5">
+        <f t="shared" si="35"/>
+        <v>7932</v>
+      </c>
+      <c r="J942" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L942" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="943" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A943">
+        <v>104529870</v>
+      </c>
+      <c r="B943" t="s">
+        <v>76</v>
+      </c>
+      <c r="C943" s="1"/>
+      <c r="E943" t="s">
+        <v>584</v>
+      </c>
+      <c r="F943" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G943">
+        <v>19566</v>
+      </c>
+      <c r="H943">
+        <v>2.27</v>
+      </c>
+      <c r="I943" s="5">
+        <f t="shared" si="35"/>
+        <v>8619.3832599118941</v>
+      </c>
+      <c r="J943" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L943" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="944" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A944">
+        <v>104527430</v>
+      </c>
+      <c r="B944" t="s">
+        <v>77</v>
+      </c>
+      <c r="C944" s="1"/>
+      <c r="E944" t="s">
+        <v>584</v>
+      </c>
+      <c r="F944" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G944">
+        <v>3070</v>
+      </c>
+      <c r="H944">
+        <v>1</v>
+      </c>
+      <c r="I944" s="5">
+        <f t="shared" si="35"/>
+        <v>3070</v>
+      </c>
+      <c r="J944" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L944" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="945" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A945">
+        <v>104529210</v>
+      </c>
+      <c r="B945" t="s">
+        <v>78</v>
+      </c>
+      <c r="C945" s="1"/>
+      <c r="E945" t="s">
+        <v>584</v>
+      </c>
+      <c r="F945" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="G945">
+        <v>4000</v>
+      </c>
+      <c r="H945">
+        <v>1</v>
+      </c>
+      <c r="I945" s="5">
+        <f t="shared" si="35"/>
+        <v>4000</v>
+      </c>
+      <c r="J945" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L945" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="946" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A946">
+        <v>104527520</v>
+      </c>
+      <c r="B946" t="s">
+        <v>79</v>
+      </c>
+      <c r="C946" s="1"/>
+      <c r="E946" t="s">
+        <v>584</v>
+      </c>
+      <c r="F946" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G946">
+        <v>3070</v>
+      </c>
+      <c r="H946">
+        <v>1</v>
+      </c>
+      <c r="I946" s="5">
+        <f t="shared" si="35"/>
+        <v>3070</v>
+      </c>
+      <c r="J946" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L946" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="947" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A947">
+        <v>104254150</v>
+      </c>
+      <c r="B947" t="s">
+        <v>81</v>
+      </c>
+      <c r="C947" s="1"/>
+      <c r="E947" t="s">
+        <v>584</v>
+      </c>
+      <c r="F947" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G947">
+        <v>22536</v>
+      </c>
+      <c r="H947">
+        <f>36 * 0.067</f>
+        <v>2.4119999999999999</v>
+      </c>
+      <c r="I947" s="5">
+        <f t="shared" si="35"/>
+        <v>9343.2835820895525</v>
+      </c>
+      <c r="J947" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L947" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="948" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A948">
+        <v>104523150</v>
+      </c>
+      <c r="B948" t="s">
+        <v>82</v>
+      </c>
+      <c r="C948" s="1"/>
+      <c r="E948" t="s">
+        <v>584</v>
+      </c>
+      <c r="F948" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="G948">
+        <v>37158</v>
+      </c>
+      <c r="H948">
+        <f>48*0.012</f>
+        <v>0.57600000000000007</v>
+      </c>
+      <c r="I948" s="5">
+        <f t="shared" si="35"/>
+        <v>64510.416666666657</v>
+      </c>
+      <c r="J948" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L948" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="949" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A949">
+        <v>104523170</v>
+      </c>
+      <c r="B949" t="s">
+        <v>83</v>
+      </c>
+      <c r="C949" s="1"/>
+      <c r="E949" t="s">
+        <v>584</v>
+      </c>
+      <c r="F949" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G949">
+        <v>27102</v>
+      </c>
+      <c r="H949">
+        <f>90*0.02</f>
+        <v>1.8</v>
+      </c>
+      <c r="I949" s="5">
+        <f t="shared" si="35"/>
+        <v>15056.666666666666</v>
+      </c>
+      <c r="J949" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L949" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="950" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A950">
+        <v>105154330</v>
+      </c>
+      <c r="B950" t="s">
+        <v>84</v>
+      </c>
+      <c r="C950" s="1"/>
+      <c r="E950" t="s">
+        <v>584</v>
+      </c>
+      <c r="F950" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="G950">
+        <v>62734</v>
+      </c>
+      <c r="H950">
+        <f>48 * 0.08</f>
+        <v>3.84</v>
+      </c>
+      <c r="I950" s="5">
+        <f t="shared" si="35"/>
+        <v>16336.979166666668</v>
+      </c>
+      <c r="J950" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L950" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="951" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A951">
+        <v>104527850</v>
+      </c>
+      <c r="B951" t="s">
+        <v>85</v>
+      </c>
+      <c r="C951" s="1"/>
+      <c r="E951" t="s">
+        <v>584</v>
+      </c>
+      <c r="F951" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G951">
+        <v>22536</v>
+      </c>
+      <c r="H951">
+        <f>36 * 0.067</f>
+        <v>2.4119999999999999</v>
+      </c>
+      <c r="I951" s="5">
+        <f t="shared" ref="I951:I993" si="36">G951/H951</f>
+        <v>9343.2835820895525</v>
+      </c>
+      <c r="J951" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L951" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="952" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A952">
+        <v>105154770</v>
+      </c>
+      <c r="B952" t="s">
+        <v>86</v>
+      </c>
+      <c r="C952" s="1"/>
+      <c r="E952" t="s">
+        <v>584</v>
+      </c>
+      <c r="F952" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G952">
+        <v>22536</v>
+      </c>
+      <c r="H952">
+        <f>36 * 0.067</f>
+        <v>2.4119999999999999</v>
+      </c>
+      <c r="I952" s="5">
+        <f t="shared" si="36"/>
+        <v>9343.2835820895525</v>
+      </c>
+      <c r="J952" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L952" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="953" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A953">
+        <v>104537940</v>
+      </c>
+      <c r="B953" t="s">
+        <v>87</v>
+      </c>
+      <c r="C953" s="1"/>
+      <c r="E953" t="s">
+        <v>584</v>
+      </c>
+      <c r="F953" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G953">
+        <v>47198</v>
+      </c>
+      <c r="H953">
+        <f>63*0.114</f>
+        <v>7.1820000000000004</v>
+      </c>
+      <c r="I953" s="5">
+        <f t="shared" si="36"/>
+        <v>6571.7070453912556</v>
+      </c>
+      <c r="J953" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L953" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="954" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A954">
+        <v>105154610</v>
+      </c>
+      <c r="B954" t="s">
+        <v>88</v>
+      </c>
+      <c r="C954" s="1"/>
+      <c r="E954" t="s">
+        <v>584</v>
+      </c>
+      <c r="F954" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G954">
+        <v>38151</v>
+      </c>
+      <c r="H954">
+        <f>14 * 0.1</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="I954" s="5">
+        <f t="shared" si="36"/>
+        <v>27250.714285714283</v>
+      </c>
+      <c r="J954" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L954" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="955" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A955">
+        <v>104521710</v>
+      </c>
+      <c r="B955" t="s">
+        <v>89</v>
+      </c>
+      <c r="C955" s="1"/>
+      <c r="E955" t="s">
+        <v>584</v>
+      </c>
+      <c r="F955" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G955">
+        <v>25195</v>
+      </c>
+      <c r="H955">
+        <f>36*0.065</f>
+        <v>2.34</v>
+      </c>
+      <c r="I955" s="5">
+        <f t="shared" si="36"/>
+        <v>10767.094017094018</v>
+      </c>
+      <c r="J955" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L955" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="956" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A956">
+        <v>104542880</v>
+      </c>
+      <c r="B956" t="s">
+        <v>91</v>
+      </c>
+      <c r="C956" s="1"/>
+      <c r="E956" t="s">
+        <v>584</v>
+      </c>
+      <c r="F956" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G956">
+        <v>16157</v>
+      </c>
+      <c r="H956">
+        <f>20*0.11</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I956" s="5">
+        <f t="shared" si="36"/>
+        <v>7344.0909090909081</v>
+      </c>
+      <c r="J956" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L956" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="957" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A957">
+        <v>104518330</v>
+      </c>
+      <c r="B957" t="s">
+        <v>93</v>
+      </c>
+      <c r="C957" s="1"/>
+      <c r="E957" t="s">
+        <v>584</v>
+      </c>
+      <c r="F957" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G957">
+        <v>35717</v>
+      </c>
+      <c r="H957">
+        <f>110 * 0.035</f>
+        <v>3.8500000000000005</v>
+      </c>
+      <c r="I957" s="5">
+        <f t="shared" si="36"/>
+        <v>9277.1428571428551</v>
+      </c>
+      <c r="J957" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L957" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="958" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A958">
+        <v>104517170</v>
+      </c>
+      <c r="B958" t="s">
+        <v>96</v>
+      </c>
+      <c r="C958" s="1"/>
+      <c r="E958" t="s">
+        <v>584</v>
+      </c>
+      <c r="F958" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G958">
+        <v>7252</v>
+      </c>
+      <c r="H958">
+        <v>0.35</v>
+      </c>
+      <c r="I958" s="5">
+        <f t="shared" si="36"/>
+        <v>20720</v>
+      </c>
+      <c r="J958" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L958" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="959" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A959">
+        <v>104521840</v>
+      </c>
+      <c r="B959" t="s">
+        <v>97</v>
+      </c>
+      <c r="C959" s="1"/>
+      <c r="E959" t="s">
+        <v>584</v>
+      </c>
+      <c r="F959" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="G959">
+        <v>71944</v>
+      </c>
+      <c r="H959">
+        <v>6.82</v>
+      </c>
+      <c r="I959" s="5">
+        <f t="shared" si="36"/>
+        <v>10548.973607038122</v>
+      </c>
+      <c r="J959" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L959" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="960" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A960">
+        <v>104534790</v>
+      </c>
+      <c r="B960" t="s">
+        <v>98</v>
+      </c>
+      <c r="C960" s="1"/>
+      <c r="E960" t="s">
+        <v>584</v>
+      </c>
+      <c r="F960" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G960">
+        <v>8591</v>
+      </c>
+      <c r="H960">
+        <v>1.36</v>
+      </c>
+      <c r="I960" s="5">
+        <f t="shared" si="36"/>
+        <v>6316.911764705882</v>
+      </c>
+      <c r="J960" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L960" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="961" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A961">
+        <v>104547160</v>
+      </c>
+      <c r="B961" t="s">
+        <v>99</v>
+      </c>
+      <c r="C961" s="1"/>
+      <c r="E961" t="s">
+        <v>584</v>
+      </c>
+      <c r="F961" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G961">
+        <v>8591</v>
+      </c>
+      <c r="H961">
+        <v>1.36</v>
+      </c>
+      <c r="I961" s="5">
+        <f t="shared" si="36"/>
+        <v>6316.911764705882</v>
+      </c>
+      <c r="J961" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L961" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="962" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A962">
+        <v>104541760</v>
+      </c>
+      <c r="B962" t="s">
+        <v>100</v>
+      </c>
+      <c r="C962" s="1"/>
+      <c r="E962" t="s">
+        <v>584</v>
+      </c>
+      <c r="F962" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G962">
+        <v>8591</v>
+      </c>
+      <c r="H962">
+        <v>1.36</v>
+      </c>
+      <c r="I962" s="5">
+        <f t="shared" si="36"/>
+        <v>6316.911764705882</v>
+      </c>
+      <c r="J962" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L962" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="963" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A963">
+        <v>104500860</v>
+      </c>
+      <c r="B963" t="s">
+        <v>104</v>
+      </c>
+      <c r="C963" s="1"/>
+      <c r="E963" t="s">
+        <v>584</v>
+      </c>
+      <c r="F963" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="G963">
+        <v>8900</v>
+      </c>
+      <c r="H963">
+        <v>5</v>
+      </c>
+      <c r="I963" s="5">
+        <f t="shared" si="36"/>
+        <v>1780</v>
+      </c>
+      <c r="J963" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L963" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="964" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A964">
+        <v>150001987</v>
+      </c>
+      <c r="B964" t="s">
+        <v>105</v>
+      </c>
+      <c r="C964" s="1"/>
+      <c r="E964" t="s">
+        <v>584</v>
+      </c>
+      <c r="F964" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G964">
+        <v>3090</v>
+      </c>
+      <c r="H964">
+        <f>_xlfn.XLOOKUP(A964,'[1]BD LP'!$B:$B,'[1]BD LP'!$AC:$AC)</f>
+        <v>1</v>
+      </c>
+      <c r="I964" s="5">
+        <f t="shared" si="36"/>
+        <v>3090</v>
+      </c>
+      <c r="J964" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L964" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="965" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A965">
+        <v>150001986</v>
+      </c>
+      <c r="B965" t="s">
+        <v>106</v>
+      </c>
+      <c r="C965" s="1"/>
+      <c r="E965" t="s">
+        <v>584</v>
+      </c>
+      <c r="F965" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="G965">
+        <v>2990</v>
+      </c>
+      <c r="H965">
+        <f>_xlfn.XLOOKUP(A965,'[1]BD LP'!$B:$B,'[1]BD LP'!$AC:$AC)</f>
+        <v>1</v>
+      </c>
+      <c r="I965" s="5">
+        <f t="shared" si="36"/>
+        <v>2990</v>
+      </c>
+      <c r="J965" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L965" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="966" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A966">
+        <v>104500730</v>
+      </c>
+      <c r="B966" t="s">
+        <v>107</v>
+      </c>
+      <c r="C966" s="1"/>
+      <c r="E966" t="s">
+        <v>584</v>
+      </c>
+      <c r="F966" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G966">
+        <v>10190</v>
+      </c>
+      <c r="H966">
+        <f>_xlfn.XLOOKUP(A966,'[1]BD LP'!$B:$B,'[1]BD LP'!$AC:$AC)</f>
+        <v>1</v>
+      </c>
+      <c r="I966" s="5">
+        <f t="shared" si="36"/>
+        <v>10190</v>
+      </c>
+      <c r="J966" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L966" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="967" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A967">
+        <v>104500760</v>
+      </c>
+      <c r="B967" t="s">
+        <v>108</v>
+      </c>
+      <c r="C967" s="1"/>
+      <c r="E967" t="s">
+        <v>584</v>
+      </c>
+      <c r="F967" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="G967">
+        <v>12090</v>
+      </c>
+      <c r="H967">
+        <f>_xlfn.XLOOKUP(A967,'[1]BD LP'!$B:$B,'[1]BD LP'!$AC:$AC)</f>
+        <v>1</v>
+      </c>
+      <c r="I967" s="5">
+        <f t="shared" si="36"/>
+        <v>12090</v>
+      </c>
+      <c r="J967" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L967" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="968" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A968">
+        <v>104500560</v>
+      </c>
+      <c r="B968" t="s">
+        <v>109</v>
+      </c>
+      <c r="C968" s="1"/>
+      <c r="E968" t="s">
+        <v>584</v>
+      </c>
+      <c r="F968" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G968">
+        <v>8590</v>
+      </c>
+      <c r="H968">
+        <f>_xlfn.XLOOKUP(A968,'[1]BD LP'!$B:$B,'[1]BD LP'!$AC:$AC)</f>
+        <v>1</v>
+      </c>
+      <c r="I968" s="5">
+        <f t="shared" si="36"/>
+        <v>8590</v>
+      </c>
+      <c r="J968" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L968" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="969" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A969">
+        <v>105045100</v>
+      </c>
+      <c r="B969" t="s">
+        <v>116</v>
+      </c>
+      <c r="C969" s="1"/>
+      <c r="E969" t="s">
+        <v>584</v>
+      </c>
+      <c r="F969" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="G969">
+        <v>14059</v>
+      </c>
+      <c r="H969">
+        <v>3</v>
+      </c>
+      <c r="I969" s="5">
+        <f t="shared" si="36"/>
+        <v>4686.333333333333</v>
+      </c>
+      <c r="J969" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L969" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="970" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A970">
+        <v>104520680</v>
+      </c>
+      <c r="B970" t="s">
+        <v>117</v>
+      </c>
+      <c r="C970" s="1"/>
+      <c r="E970" t="s">
+        <v>584</v>
+      </c>
+      <c r="F970" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="G970">
+        <v>10212</v>
+      </c>
+      <c r="H970">
+        <v>3</v>
+      </c>
+      <c r="I970" s="5">
+        <f t="shared" si="36"/>
+        <v>3404</v>
+      </c>
+      <c r="J970" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L970" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="971" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A971">
+        <v>104538110</v>
+      </c>
+      <c r="B971" t="s">
+        <v>119</v>
+      </c>
+      <c r="C971" s="1"/>
+      <c r="E971" t="s">
+        <v>584</v>
+      </c>
+      <c r="F971" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G971">
+        <v>1535</v>
+      </c>
+      <c r="H971">
+        <v>0.93</v>
+      </c>
+      <c r="I971" s="5">
+        <f t="shared" si="36"/>
+        <v>1650.5376344086021</v>
+      </c>
+      <c r="J971" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L971" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="972" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A972">
+        <v>201200013</v>
+      </c>
+      <c r="B972" t="s">
+        <v>120</v>
+      </c>
+      <c r="C972" s="1"/>
+      <c r="E972" t="s">
+        <v>584</v>
+      </c>
+      <c r="F972" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G972">
+        <v>1535</v>
+      </c>
+      <c r="H972">
+        <v>0.93</v>
+      </c>
+      <c r="I972" s="5">
+        <f t="shared" si="36"/>
+        <v>1650.5376344086021</v>
+      </c>
+      <c r="J972" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L972" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="973" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A973">
+        <v>104528900</v>
+      </c>
+      <c r="B973" t="s">
+        <v>121</v>
+      </c>
+      <c r="E973" t="s">
+        <v>584</v>
+      </c>
+      <c r="F973" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="G973">
+        <v>3090</v>
+      </c>
+      <c r="H973">
+        <v>1</v>
+      </c>
+      <c r="I973" s="5">
+        <f t="shared" si="36"/>
+        <v>3090</v>
+      </c>
+      <c r="J973" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L973" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="974" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A974">
+        <v>104530290</v>
+      </c>
+      <c r="B974" t="s">
+        <v>122</v>
+      </c>
+      <c r="E974" t="s">
+        <v>584</v>
+      </c>
+      <c r="F974" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="G974">
+        <v>16114</v>
+      </c>
+      <c r="H974">
+        <v>3.78</v>
+      </c>
+      <c r="I974" s="5">
+        <f t="shared" si="36"/>
+        <v>4262.9629629629635</v>
+      </c>
+      <c r="J974" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L974" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="975" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A975">
+        <v>150000140</v>
+      </c>
+      <c r="B975" t="s">
+        <v>123</v>
+      </c>
+      <c r="E975" t="s">
+        <v>584</v>
+      </c>
+      <c r="F975" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="G975">
+        <v>5373</v>
+      </c>
+      <c r="H975">
+        <v>1.94</v>
+      </c>
+      <c r="I975" s="5">
+        <f t="shared" si="36"/>
+        <v>2769.5876288659792</v>
+      </c>
+      <c r="J975" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L975" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="976" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A976">
+        <v>150001952</v>
+      </c>
+      <c r="B976" t="s">
+        <v>125</v>
+      </c>
+      <c r="E976" t="s">
+        <v>584</v>
+      </c>
+      <c r="F976" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="G976">
+        <v>7390</v>
+      </c>
+      <c r="H976">
+        <v>1</v>
+      </c>
+      <c r="I976" s="5">
+        <f t="shared" si="36"/>
+        <v>7390</v>
+      </c>
+      <c r="J976" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L976" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="977" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A977">
+        <v>104515580</v>
+      </c>
+      <c r="B977" t="s">
+        <v>127</v>
+      </c>
+      <c r="E977" t="s">
+        <v>584</v>
+      </c>
+      <c r="F977" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G977">
+        <v>55919</v>
+      </c>
+      <c r="H977">
+        <f>60*0.08</f>
+        <v>4.8</v>
+      </c>
+      <c r="I977" s="5">
+        <f t="shared" si="36"/>
+        <v>11649.791666666668</v>
+      </c>
+      <c r="J977" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L977" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="978" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A978">
+        <v>104528980</v>
+      </c>
+      <c r="B978" t="s">
+        <v>129</v>
+      </c>
+      <c r="E978" t="s">
+        <v>584</v>
+      </c>
+      <c r="F978" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G978">
+        <v>27057</v>
+      </c>
+      <c r="H978">
+        <f>180*0.045</f>
+        <v>8.1</v>
+      </c>
+      <c r="I978" s="5">
+        <f t="shared" si="36"/>
+        <v>3340.3703703703704</v>
+      </c>
+      <c r="J978" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L978" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="979" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A979">
+        <v>104528990</v>
+      </c>
+      <c r="B979" t="s">
+        <v>130</v>
+      </c>
+      <c r="E979" t="s">
+        <v>584</v>
+      </c>
+      <c r="F979" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G979">
+        <v>27057</v>
+      </c>
+      <c r="H979">
+        <f>180*0.045</f>
+        <v>8.1</v>
+      </c>
+      <c r="I979" s="5">
+        <f t="shared" si="36"/>
+        <v>3340.3703703703704</v>
+      </c>
+      <c r="J979" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L979" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="980" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A980">
+        <v>101520140</v>
+      </c>
+      <c r="B980" t="s">
+        <v>132</v>
+      </c>
+      <c r="E980" t="s">
+        <v>584</v>
+      </c>
+      <c r="F980" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="G980">
+        <v>3761</v>
+      </c>
+      <c r="H980">
+        <f>0.8</f>
+        <v>0.8</v>
+      </c>
+      <c r="I980" s="5">
+        <f t="shared" si="36"/>
+        <v>4701.25</v>
+      </c>
+      <c r="J980" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L980" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="981" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A981">
+        <v>101500120</v>
+      </c>
+      <c r="B981" t="s">
+        <v>133</v>
+      </c>
+      <c r="E981" t="s">
+        <v>584</v>
+      </c>
+      <c r="F981" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G981">
+        <v>7429</v>
+      </c>
+      <c r="H981">
+        <v>2.84</v>
+      </c>
+      <c r="I981" s="5">
+        <f t="shared" si="36"/>
+        <v>2615.8450704225352</v>
+      </c>
+      <c r="J981" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L981" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="982" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A982">
+        <v>104542770</v>
+      </c>
+      <c r="B982" t="s">
+        <v>135</v>
+      </c>
+      <c r="E982" t="s">
+        <v>584</v>
+      </c>
+      <c r="F982" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="G982">
+        <v>4672</v>
+      </c>
+      <c r="H982">
+        <v>1</v>
+      </c>
+      <c r="I982" s="5">
+        <f t="shared" si="36"/>
+        <v>4672</v>
+      </c>
+      <c r="J982" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L982" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="983" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A983">
+        <v>101520250</v>
+      </c>
+      <c r="B983" t="s">
+        <v>136</v>
+      </c>
+      <c r="E983" t="s">
+        <v>584</v>
+      </c>
+      <c r="F983" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G983">
+        <v>1975</v>
+      </c>
+      <c r="H983">
+        <v>0.8</v>
+      </c>
+      <c r="I983" s="5">
+        <f t="shared" si="36"/>
+        <v>2468.75</v>
+      </c>
+      <c r="J983" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L983" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="984" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A984">
+        <v>104534690</v>
+      </c>
+      <c r="B984" t="s">
+        <v>137</v>
+      </c>
+      <c r="E984" t="s">
+        <v>584</v>
+      </c>
+      <c r="F984" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G984">
+        <v>7429</v>
+      </c>
+      <c r="H984">
+        <v>2.84</v>
+      </c>
+      <c r="I984" s="5">
+        <f t="shared" si="36"/>
+        <v>2615.8450704225352</v>
+      </c>
+      <c r="J984" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L984" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="985" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A985">
+        <v>104519180</v>
+      </c>
+      <c r="B985" t="s">
+        <v>138</v>
+      </c>
+      <c r="E985" t="s">
+        <v>584</v>
+      </c>
+      <c r="F985" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G985">
+        <v>32850</v>
+      </c>
+      <c r="H985">
+        <f>_xlfn.XLOOKUP(A985,'[1]BD LP'!$B:$B,'[1]BD LP'!$AC:$AC)</f>
+        <v>15</v>
+      </c>
+      <c r="I985" s="5">
+        <f t="shared" si="36"/>
+        <v>2190</v>
+      </c>
+      <c r="J985" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L985" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="986" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A986">
+        <v>104522620</v>
+      </c>
+      <c r="B986" t="s">
+        <v>139</v>
+      </c>
+      <c r="E986" t="s">
+        <v>584</v>
+      </c>
+      <c r="F986" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G986">
+        <v>30350</v>
+      </c>
+      <c r="H986">
+        <f>_xlfn.XLOOKUP(A986,'[1]BD LP'!$B:$B,'[1]BD LP'!$AC:$AC)</f>
+        <v>15</v>
+      </c>
+      <c r="I986" s="5">
+        <f t="shared" si="36"/>
+        <v>2023.3333333333333</v>
+      </c>
+      <c r="J986" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L986" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="987" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A987">
+        <v>104521720</v>
+      </c>
+      <c r="B987" t="s">
+        <v>140</v>
+      </c>
+      <c r="E987" t="s">
+        <v>584</v>
+      </c>
+      <c r="F987" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="G987">
+        <v>48308</v>
+      </c>
+      <c r="H987">
+        <f>140*0.1</f>
+        <v>14</v>
+      </c>
+      <c r="I987" s="5">
+        <f t="shared" si="36"/>
+        <v>3450.5714285714284</v>
+      </c>
+      <c r="J987" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L987" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="988" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A988">
+        <v>104531370</v>
+      </c>
+      <c r="B988" t="s">
+        <v>144</v>
+      </c>
+      <c r="E988" t="s">
+        <v>584</v>
+      </c>
+      <c r="F988" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G988">
+        <v>1165</v>
+      </c>
+      <c r="H988">
+        <v>0.105</v>
+      </c>
+      <c r="I988" s="5">
+        <f t="shared" si="36"/>
+        <v>11095.238095238095</v>
+      </c>
+      <c r="J988" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L988" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="989" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A989">
+        <v>104519090</v>
+      </c>
+      <c r="B989" t="s">
+        <v>146</v>
+      </c>
+      <c r="E989" t="s">
+        <v>584</v>
+      </c>
+      <c r="F989" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="G989">
+        <v>11921</v>
+      </c>
+      <c r="H989">
+        <v>1</v>
+      </c>
+      <c r="I989" s="5">
+        <f t="shared" si="36"/>
+        <v>11921</v>
+      </c>
+      <c r="J989" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L989" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="990" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A990">
+        <v>104529560</v>
+      </c>
+      <c r="B990" t="s">
+        <v>147</v>
+      </c>
+      <c r="E990" t="s">
+        <v>584</v>
+      </c>
+      <c r="F990" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="G990">
+        <v>3921</v>
+      </c>
+      <c r="H990">
+        <v>0.2</v>
+      </c>
+      <c r="I990" s="5">
+        <f t="shared" si="36"/>
+        <v>19605</v>
+      </c>
+      <c r="J990" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L990" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="991" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A991">
+        <v>104516010</v>
+      </c>
+      <c r="B991" t="s">
+        <v>150</v>
+      </c>
+      <c r="E991" t="s">
+        <v>584</v>
+      </c>
+      <c r="F991" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="G991">
+        <v>5321</v>
+      </c>
+      <c r="H991">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="I991" s="5">
+        <f t="shared" si="36"/>
+        <v>5690.909090909091</v>
+      </c>
+      <c r="J991" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L991" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="992" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A992">
+        <v>105045700</v>
+      </c>
+      <c r="B992" t="s">
+        <v>153</v>
+      </c>
+      <c r="E992" t="s">
+        <v>584</v>
+      </c>
+      <c r="F992" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G992">
+        <v>5573</v>
+      </c>
+      <c r="H992">
+        <v>1</v>
+      </c>
+      <c r="I992" s="5">
+        <f t="shared" si="36"/>
+        <v>5573</v>
+      </c>
+      <c r="J992" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L992" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="993" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A993">
+        <v>104521670</v>
+      </c>
+      <c r="B993" t="s">
+        <v>154</v>
+      </c>
+      <c r="E993" t="s">
+        <v>584</v>
+      </c>
+      <c r="F993" s="8" t="s">
+        <v>1111</v>
+      </c>
+      <c r="G993">
+        <v>51129</v>
+      </c>
+      <c r="H993">
+        <f>_xlfn.XLOOKUP(A993,'[1]BD LP'!$B:$B,'[1]BD LP'!$AC:$AC)</f>
+        <v>5</v>
+      </c>
+      <c r="I993" s="5">
+        <f t="shared" si="36"/>
+        <v>10225.799999999999</v>
+      </c>
+      <c r="J993" s="3">
+        <v>45960</v>
+      </c>
+      <c r="L993" t="s">
+        <v>1067</v>
       </c>
     </row>
   </sheetData>
@@ -51816,6 +53626,7 @@
     <hyperlink ref="F750" r:id="rId28" xr:uid="{16346C42-021B-45FA-85D6-AD169A04B8D1}"/>
     <hyperlink ref="F854" r:id="rId29" xr:uid="{8A2D51DB-1012-45C9-8F77-6D8F57DB8B97}"/>
     <hyperlink ref="F861" r:id="rId30" xr:uid="{3FDCE067-1172-4003-9A7F-153BE51D0433}"/>
+    <hyperlink ref="F993" r:id="rId31" location="/products/detail/200300002" xr:uid="{D6E1DB14-B0CA-462C-A8EF-80CACE2FEACF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   base.xlsx 	modified:   maestro_skus.xlsx
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icbfsfood-my.sharepoint.com/personal/scatalanv_icbfs_cl/Documents/posicionamiento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6228" documentId="11_AD4D2F04E46CFB4ACB3E200E4DD7FD88683EDF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ACB1890-DFCC-476D-B4A1-2833A253B03B}"/>
+  <xr:revisionPtr revIDLastSave="6237" documentId="11_AD4D2F04E46CFB4ACB3E200E4DD7FD88683EDF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFDAE5BC-53FC-4039-9DF2-AA49113F4F14}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3841,7 +3841,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3869,6 +3869,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3901,7 +3908,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3919,6 +3926,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -23344,7 +23352,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H121" sqref="H121"/>
+      <selection pane="bottomLeft" activeCell="A325" sqref="A325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33771,8 +33779,8 @@
       </c>
     </row>
     <row r="325" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A325">
-        <v>104539700</v>
+      <c r="A325" s="9">
+        <v>150001954</v>
       </c>
       <c r="B325" t="s">
         <v>380</v>
@@ -33783,20 +33791,18 @@
       <c r="F325" s="1" t="s">
         <v>980</v>
       </c>
-      <c r="G325" t="e">
-        <f>_xlfn.XLOOKUP(A325,'[1]BD LP'!$B:$B,'[1]BD LP'!$Y:$Y)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H325" t="e">
-        <f>_xlfn.XLOOKUP(A325,'[1]BD LP'!$B:$B,'[1]BD LP'!$AC:$AC)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I325" s="5" t="e">
+      <c r="G325">
+        <v>7390</v>
+      </c>
+      <c r="H325">
+        <v>1</v>
+      </c>
+      <c r="I325" s="5">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>7390</v>
       </c>
       <c r="J325" s="3">
-        <v>45947</v>
+        <v>45979</v>
       </c>
       <c r="L325" t="s">
         <v>980</v>
@@ -47943,8 +47949,8 @@
       </c>
     </row>
     <row r="808" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A808">
-        <v>104539700</v>
+      <c r="A808" s="9">
+        <v>150001954</v>
       </c>
       <c r="B808" t="s">
         <v>904</v>

</xml_diff>